<commit_message>
Updated IND model - 2025-07-31 22:57
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_IND/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D3B86D-5E44-469A-9BFD-27A22346152F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AD581D-C637-43E8-9A19-5097D8EA4F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="145">
   <si>
     <t>Unit</t>
   </si>
@@ -115,9 +115,6 @@
     <t>TS</t>
   </si>
   <si>
-    <t>ELC</t>
-  </si>
-  <si>
     <t>VAR_CAP</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
     <t>c_neg_andor</t>
   </si>
   <si>
-    <t>ELE,STG</t>
-  </si>
-  <si>
     <t>Elec New Capacity</t>
   </si>
   <si>
@@ -472,9 +466,6 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>-ElcAgg*</t>
-  </si>
-  <si>
     <t>p,t</t>
   </si>
   <si>
@@ -506,6 +497,24 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Trd*</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>ELE,STG,IRE</t>
+  </si>
+  <si>
+    <t>ELE,IRE</t>
+  </si>
+  <si>
+    <t>-ElcAgg*,-*EV*</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???</t>
   </si>
 </sst>
 </file>
@@ -1069,55 +1078,55 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="I2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
         <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
       </c>
       <c r="M2" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1126,10 +1135,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" t="str">
         <f>"sg_"&amp;I2</f>
@@ -1174,7 +1183,7 @@
         <v>Fixed</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1202,7 +1211,7 @@
         <v>V1G</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -1230,7 +1239,7 @@
         <v>V2G</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O8">
         <v>3</v>
@@ -1256,18 +1265,18 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1276,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1314,32 +1323,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <f>1/8.76</f>
@@ -1348,13 +1357,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -1371,9 +1380,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -1404,39 +1413,39 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
@@ -1445,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -1454,56 +1463,62 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
       <c r="N3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" t="s">
-        <v>104</v>
-      </c>
-      <c r="P4" t="s">
-        <v>46</v>
-      </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U4" s="8"/>
     </row>
@@ -1511,125 +1526,134 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" t="s">
         <v>78</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" t="s">
-        <v>79</v>
-      </c>
       <c r="Q6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" t="s">
         <v>38</v>
-      </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" t="s">
-        <v>107</v>
-      </c>
-      <c r="P7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" t="s">
         <v>62</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>63</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" t="s">
         <v>65</v>
       </c>
-      <c r="K9" t="s">
-        <v>109</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" t="s">
         <v>66</v>
-      </c>
-      <c r="P9" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8EC7F-95E3-4526-8B78-C58A96098159}">
   <dimension ref="C1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1664,15 +1688,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -1681,42 +1705,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1744,18 +1768,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1779,18 +1803,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1818,18 +1842,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1854,18 +1878,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1875,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1893,71 +1917,71 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>91</v>
-      </c>
-      <c r="G2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="str">
         <f>D3</f>
         <v>CCGT</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C20" si="0">D4</f>
         <v>Int Comb</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>Gas_Oil Steam</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1969,67 +1993,67 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>OCGT (Peaker)</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Subcritical Coal</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Supercritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>IGCC</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Bioenergy</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2041,43 +2065,43 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Wind onshore</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Wind offshore</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Geothermal</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2089,7 +2113,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2101,46 +2125,46 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Hydro pumped stg</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Util Batt Stg</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>EV Batt</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2148,13 +2172,24 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2182,33 +2217,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
         <v>98</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>99</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>101</v>
-      </c>
-      <c r="G2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 13:17
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_IND/ReportDefs_vervestacks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\VerveStacks_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66696D83-239C-479D-A819-82C6ECB63F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46E727C-16A5-4FE2-B423-5DFB107A44BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3353" yWindow="1710" windowWidth="21600" windowHeight="12188" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="154">
   <si>
     <t>Unit</t>
   </si>
@@ -100,15 +100,9 @@
     <t>Solar</t>
   </si>
   <si>
-    <t>Nuc</t>
-  </si>
-  <si>
     <t>Varbl</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>VAR_FOUT</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>Ldesc</t>
   </si>
   <si>
-    <t>ProcOrd</t>
-  </si>
-  <si>
     <t>Attribute</t>
   </si>
   <si>
@@ -223,24 +214,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Shale</t>
-  </si>
-  <si>
-    <t>RECost</t>
-  </si>
-  <si>
-    <t>Re</t>
-  </si>
-  <si>
-    <t>Rg</t>
-  </si>
-  <si>
-    <t>Regions</t>
-  </si>
-  <si>
     <t>~ATS</t>
   </si>
   <si>
@@ -322,21 +295,6 @@
     <t>LCOE</t>
   </si>
   <si>
-    <t>V2G</t>
-  </si>
-  <si>
-    <t>EVCharge</t>
-  </si>
-  <si>
-    <t>trastg~</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>V1G</t>
-  </si>
-  <si>
     <t>~ScenMap</t>
   </si>
   <si>
@@ -530,6 +488,60 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>vstacks_t1~</t>
+  </si>
+  <si>
+    <t>vstacks_t5~</t>
+  </si>
+  <si>
+    <t>vstacks_w2~</t>
+  </si>
+  <si>
+    <t>ngfs</t>
+  </si>
+  <si>
+    <t>timeslice</t>
+  </si>
+  <si>
+    <t>Delayed transition</t>
+  </si>
+  <si>
+    <t>Net Zero 2050</t>
+  </si>
+  <si>
+    <t>Current Policies</t>
+  </si>
+  <si>
+    <t>Low demand</t>
+  </si>
+  <si>
+    <t>Fragmented World</t>
+  </si>
+  <si>
+    <t>NDCs</t>
+  </si>
+  <si>
+    <t>Below 2deg</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>15 days</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>_3d</t>
+  </si>
+  <si>
+    <t>_15d</t>
+  </si>
+  <si>
+    <t>_2w</t>
   </si>
 </sst>
 </file>
@@ -1068,196 +1080,652 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.73046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>136</v>
+      </c>
       <c r="B1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="H2" t="s">
+        <v>139</v>
+      </c>
       <c r="I2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>71</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="str">
+        <f>"sg_"&amp;H2</f>
+        <v>sg_ngfs</v>
       </c>
       <c r="I5" t="str">
         <f>"sg_"&amp;I2</f>
-        <v>sg_EVCharge</v>
-      </c>
-      <c r="K5" t="str">
-        <f>"sg_"&amp;K2</f>
-        <v>sg_Shale</v>
-      </c>
-      <c r="L5" t="str">
-        <f>"sg_"&amp;L2</f>
-        <v>sg_RECost</v>
-      </c>
-      <c r="M5" t="str">
-        <f>"sg_"&amp;M2</f>
-        <v>sg_Nuc</v>
-      </c>
-      <c r="N5" t="str">
-        <f>"sg_"&amp;N2</f>
-        <v>sg_Regions</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>sg_timeslice</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="str">
+        <f>$A$1&amp;TEXT(N6,"0000")</f>
+        <v>vstacks_t1~0001</v>
+      </c>
       <c r="B6" t="str">
-        <f>$B$1&amp;TEXT(O6,"0000")</f>
-        <v>trastg~0001</v>
-      </c>
-      <c r="C6" t="str">
+        <f>G6</f>
+        <v>Delayed transition_3d</v>
+      </c>
+      <c r="G6" t="str">
+        <f>H6&amp;P6</f>
+        <v>Delayed transition_3d</v>
+      </c>
+      <c r="H6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" t="s">
+        <v>148</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="str">
+        <f t="shared" ref="A7:A26" si="0">$A$1&amp;TEXT(N7,"0000")</f>
+        <v>vstacks_t1~0002</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ref="B7:B26" si="1">G7</f>
+        <v>Net Zero 2050_3d</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ref="G7:G26" si="2">H7&amp;P7</f>
+        <v>Net Zero 2050_3d</v>
+      </c>
+      <c r="H7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" t="s">
+        <v>148</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_t1~0003</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="1"/>
+        <v>NDCs_3d</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>NDCs_3d</v>
+      </c>
+      <c r="H8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I8" t="s">
+        <v>148</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_t1~0004</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="1"/>
+        <v>Below 2deg_3d</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>Below 2deg_3d</v>
+      </c>
+      <c r="H9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9" t="s">
+        <v>148</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="P9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_t1~0005</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="1"/>
+        <v>Current Policies_3d</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>Current Policies_3d</v>
+      </c>
+      <c r="H10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" t="s">
+        <v>148</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_t1~0006</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="1"/>
+        <v>Low demand_3d</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>Low demand_3d</v>
+      </c>
+      <c r="H11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="P11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_t1~0007</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v>Fragmented World_3d</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>Fragmented World_3d</v>
+      </c>
+      <c r="H12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I12" t="s">
+        <v>148</v>
+      </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
+      <c r="P12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="str">
+        <f>$B$1&amp;TEXT(N13,"0000")</f>
+        <v>vstacks_t5~0001</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v>Delayed transition_15d</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>Delayed transition_15d</v>
+      </c>
+      <c r="H13" t="str">
         <f>H6</f>
-        <v>Fixed</v>
-      </c>
-      <c r="D6" t="str">
-        <f>C6</f>
-        <v>Fixed</v>
-      </c>
-      <c r="E6" t="str">
-        <f>D6</f>
-        <v>Fixed</v>
-      </c>
-      <c r="H6" t="str">
-        <f>I6</f>
-        <v>Fixed</v>
-      </c>
-      <c r="I6" t="s">
-        <v>83</v>
-      </c>
-      <c r="O6">
+        <v>Delayed transition</v>
+      </c>
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+      <c r="N13">
+        <f>N6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="B7" t="str">
-        <f t="shared" ref="B7:B8" si="0">$B$1&amp;TEXT(O7,"0000")</f>
-        <v>trastg~0002</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" ref="C7:C8" si="1">H7</f>
-        <v>V1G</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" ref="D7:E7" si="2">C7</f>
-        <v>V1G</v>
-      </c>
-      <c r="E7" t="str">
+      <c r="P13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="str">
+        <f t="shared" ref="A14:A26" si="3">$B$1&amp;TEXT(N14,"0000")</f>
+        <v>vstacks_t5~0002</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>Net Zero 2050_15d</v>
+      </c>
+      <c r="G14" t="str">
         <f t="shared" si="2"/>
-        <v>V1G</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" ref="H7:H8" si="3">I7</f>
-        <v>V1G</v>
-      </c>
-      <c r="I7" t="s">
-        <v>84</v>
-      </c>
-      <c r="O7">
+        <v>Net Zero 2050_15d</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" ref="H14:H26" si="4">H7</f>
+        <v>Net Zero 2050</v>
+      </c>
+      <c r="I14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14:N26" si="5">N7</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>trastg~0003</v>
-      </c>
-      <c r="C8" t="str">
+      <c r="P14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="str">
+        <f t="shared" si="3"/>
+        <v>vstacks_t5~0003</v>
+      </c>
+      <c r="B15" t="str">
         <f t="shared" si="1"/>
-        <v>V2G</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" ref="D8:E8" si="4">C8</f>
-        <v>V2G</v>
-      </c>
-      <c r="E8" t="str">
+        <v>NDCs_15d</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>NDCs_15d</v>
+      </c>
+      <c r="H15" t="str">
         <f t="shared" si="4"/>
-        <v>V2G</v>
-      </c>
-      <c r="H8" t="str">
+        <v>NDCs</v>
+      </c>
+      <c r="I15" t="s">
+        <v>149</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="str">
         <f t="shared" si="3"/>
-        <v>V2G</v>
-      </c>
-      <c r="I8" t="s">
-        <v>80</v>
-      </c>
-      <c r="O8">
+        <v>vstacks_t5~0004</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>Below 2deg_15d</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>Below 2deg_15d</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="4"/>
+        <v>Below 2deg</v>
+      </c>
+      <c r="I16" t="s">
+        <v>149</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="str">
+        <f t="shared" si="3"/>
+        <v>vstacks_t5~0005</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="1"/>
+        <v>Current Policies_15d</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v>Current Policies_15d</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="4"/>
+        <v>Current Policies</v>
+      </c>
+      <c r="I17" t="s">
+        <v>149</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="str">
+        <f t="shared" si="3"/>
+        <v>vstacks_t5~0006</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="1"/>
+        <v>Low demand_15d</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>Low demand_15d</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="4"/>
+        <v>Low demand</v>
+      </c>
+      <c r="I18" t="s">
+        <v>149</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="str">
+        <f t="shared" si="3"/>
+        <v>vstacks_t5~0007</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="1"/>
+        <v>Fragmented World_15d</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>Fragmented World_15d</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="4"/>
+        <v>Fragmented World</v>
+      </c>
+      <c r="I19" t="s">
+        <v>149</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="str">
+        <f>$C$1&amp;TEXT(N20,"0000")</f>
+        <v>vstacks_w2~0001</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="1"/>
+        <v>Delayed transition_2w</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>Delayed transition_2w</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="4"/>
+        <v>Delayed transition</v>
+      </c>
+      <c r="I20" t="s">
+        <v>150</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="str">
+        <f t="shared" ref="A21:A26" si="6">$C$1&amp;TEXT(N21,"0000")</f>
+        <v>vstacks_w2~0002</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="1"/>
+        <v>Net Zero 2050_2w</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>Net Zero 2050_2w</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="4"/>
+        <v>Net Zero 2050</v>
+      </c>
+      <c r="I21" t="s">
+        <v>150</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="str">
+        <f t="shared" si="6"/>
+        <v>vstacks_w2~0003</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="1"/>
+        <v>NDCs_2w</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>NDCs_2w</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="4"/>
+        <v>NDCs</v>
+      </c>
+      <c r="I22" t="s">
+        <v>150</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="5"/>
         <v>3</v>
+      </c>
+      <c r="P22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="str">
+        <f t="shared" si="6"/>
+        <v>vstacks_w2~0004</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="1"/>
+        <v>Below 2deg_2w</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>Below 2deg_2w</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="4"/>
+        <v>Below 2deg</v>
+      </c>
+      <c r="I23" t="s">
+        <v>150</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="str">
+        <f t="shared" si="6"/>
+        <v>vstacks_w2~0005</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="1"/>
+        <v>Current Policies_2w</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>Current Policies_2w</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="4"/>
+        <v>Current Policies</v>
+      </c>
+      <c r="I24" t="s">
+        <v>150</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="str">
+        <f t="shared" si="6"/>
+        <v>vstacks_w2~0006</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>Low demand_2w</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>Low demand_2w</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="4"/>
+        <v>Low demand</v>
+      </c>
+      <c r="I25" t="s">
+        <v>150</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="str">
+        <f t="shared" si="6"/>
+        <v>vstacks_w2~0007</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="1"/>
+        <v>Fragmented World_2w</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>Fragmented World_2w</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="4"/>
+        <v>Fragmented World</v>
+      </c>
+      <c r="I26" t="s">
+        <v>150</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P26" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1280,30 +1748,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1338,32 +1806,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <f>1/8.76</f>
@@ -1372,13 +1840,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -1395,7 +1863,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
@@ -1428,48 +1896,48 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -1478,197 +1946,197 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="P3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="K4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="P4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="I5" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="K5" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="N5" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="P5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="K6" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="N6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="P6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="Q6" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="N7" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="P7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="N8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="P8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="Q8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K9" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="N9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="P9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="Q9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K10" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="N10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="Q10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1703,15 +2171,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -1720,42 +2188,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="J2" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I3" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1783,18 +2251,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1818,18 +2286,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1857,18 +2325,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1893,18 +2361,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1916,7 +2384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1932,71 +2400,71 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C3" t="str">
         <f>D3</f>
         <v>CCGT</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C20" si="0">D4</f>
         <v>Int Comb</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>Gas_Oil Steam</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -2008,67 +2476,67 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>OCGT (Peaker)</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Subcritical Coal</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Supercritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>IGCC</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Bioenergy</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2080,43 +2548,43 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Wind onshore</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Wind offshore</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Geothermal</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2128,7 +2596,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2140,46 +2608,46 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Hydro pumped stg</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Util Batt Stg</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>EV Batt</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2187,46 +2655,46 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2254,33 +2722,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated IND model - 2025-09-04 01:01
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_IND/ReportDefs_vervestacks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DDB825-DE2D-493C-BFA9-B4AB649A3FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4042D569-A5F5-4C9A-B6BD-B6761B7C14D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="293">
   <si>
     <t>Unit</t>
   </si>
@@ -500,9 +500,6 @@
     <t>gas</t>
   </si>
   <si>
-    <t>co2captured</t>
-  </si>
-  <si>
     <t>*ccs-rf</t>
   </si>
   <si>
@@ -563,18 +560,12 @@
     <t>-ElcAgg*,-*EV*,-g[_]*</t>
   </si>
   <si>
-    <t>ELC,ELC_???-???,e[_]*</t>
-  </si>
-  <si>
     <t>T_neg_andor</t>
   </si>
   <si>
     <t>downscale_option</t>
   </si>
   <si>
-    <t>~TS_Defs: Snk_attr=Grid Flows</t>
-  </si>
-  <si>
     <t>TWh</t>
   </si>
   <si>
@@ -876,6 +867,99 @@
   </si>
   <si>
     <t>ar6_r10</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???*,e[_]*</t>
+  </si>
+  <si>
+    <t>*ccs</t>
+  </si>
+  <si>
+    <t>s1_d</t>
+  </si>
+  <si>
+    <t>f3d</t>
+  </si>
+  <si>
+    <t>~TS_Defs: Snk_attr=SANKEY Grid Flows</t>
+  </si>
+  <si>
+    <t>~TS_Defs: Snk_attr=SANKEY whole system</t>
+  </si>
+  <si>
+    <t>geothermal</t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>windon</t>
+  </si>
+  <si>
+    <t>windoff</t>
+  </si>
+  <si>
+    <t>wind onshore</t>
+  </si>
+  <si>
+    <t>wind offshore</t>
+  </si>
+  <si>
+    <t>&lt;gen_cname&gt;_src_&lt;gen_pname&gt;</t>
+  </si>
+  <si>
+    <t>&lt;gen_cname&gt;_snk_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>&lt;gen_cname&gt;_snk_&lt;gen_pname&gt;</t>
+  </si>
+  <si>
+    <t>Fuels</t>
+  </si>
+  <si>
+    <t>Onshore Wind</t>
+  </si>
+  <si>
+    <t>Offshore Wind</t>
+  </si>
+  <si>
+    <t>f*</t>
+  </si>
+  <si>
+    <t>NatGas_src_&lt;gen_pname&gt;</t>
+  </si>
+  <si>
+    <t>NatGas_snk_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>&lt;cset&gt;_src_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>&lt;cset&gt;_snk_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>ELC,ELC[_]spv*,ELC[_]wo*</t>
+  </si>
+  <si>
+    <t>Electricity_src_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>Electricity_snk_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>&lt;cset&gt;_snk_&lt;gen_pname&gt;</t>
   </si>
 </sst>
 </file>
@@ -1420,11 +1504,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:U55"/>
+  <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
   <cols>
@@ -1446,7 +1528,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="I2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J2" t="s">
         <v>125</v>
@@ -1505,14 +1587,14 @@
         <v>e 1.5 deg no OS.e3d</v>
       </c>
       <c r="I6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J6" t="str">
         <f>Q6</f>
         <v>e3d</v>
       </c>
       <c r="L6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1525,10 +1607,10 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="U6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1548,14 +1630,14 @@
         <v>d 1.5 deg OS.e3d</v>
       </c>
       <c r="I7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" ref="J7:J55" si="3">Q7</f>
         <v>e3d</v>
       </c>
       <c r="L7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -1568,10 +1650,10 @@
         <v>2</v>
       </c>
       <c r="T7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="U7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1591,14 +1673,14 @@
         <v>c 2 deg (67%).e3d</v>
       </c>
       <c r="I8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="3"/>
         <v>e3d</v>
       </c>
       <c r="L8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O8">
         <v>3</v>
@@ -1611,10 +1693,10 @@
         <v>3</v>
       </c>
       <c r="T8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="U8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1634,14 +1716,14 @@
         <v>b 2 deg (50%).e3d</v>
       </c>
       <c r="I9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="3"/>
         <v>e3d</v>
       </c>
       <c r="L9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="O9">
         <v>4</v>
@@ -1654,10 +1736,10 @@
         <v>4</v>
       </c>
       <c r="T9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="U9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1677,14 +1759,14 @@
         <v>a 3 deg.e3d</v>
       </c>
       <c r="I10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="3"/>
         <v>e3d</v>
       </c>
       <c r="L10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="O10">
         <v>5</v>
@@ -1697,10 +1779,10 @@
         <v>5</v>
       </c>
       <c r="T10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="U10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1740,15 +1822,15 @@
         <v>6</v>
       </c>
       <c r="T11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="U11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12">
-        <f t="shared" ref="A12:A55" si="5">A7+1</f>
+        <f t="shared" ref="A12:A60" si="5">A7+1</f>
         <v>2</v>
       </c>
       <c r="B12" t="str">
@@ -1764,7 +1846,7 @@
         <v>d 1.5 deg OS.d9d</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" ref="I12:I55" si="6">I7</f>
+        <f t="shared" ref="I12:I60" si="6">I7</f>
         <v>d 1.5 deg OS</v>
       </c>
       <c r="J12" t="str">
@@ -1772,7 +1854,7 @@
         <v>d9d</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O55" si="7">O7</f>
+        <f t="shared" ref="O12:O60" si="7">O7</f>
         <v>2</v>
       </c>
       <c r="Q12" t="str">
@@ -1783,10 +1865,10 @@
         <v>7</v>
       </c>
       <c r="T12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="U12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1826,10 +1908,10 @@
         <v>8</v>
       </c>
       <c r="T13" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="U13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1869,10 +1951,10 @@
         <v>9</v>
       </c>
       <c r="T14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="U14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1912,10 +1994,10 @@
         <v>10</v>
       </c>
       <c r="T15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="U15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1951,6 +2033,15 @@
         <f t="shared" si="4"/>
         <v>b2w</v>
       </c>
+      <c r="S16">
+        <v>11</v>
+      </c>
+      <c r="T16" t="s">
+        <v>264</v>
+      </c>
+      <c r="U16" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17">
@@ -3276,6 +3367,176 @@
       <c r="Q55" t="str">
         <f t="shared" si="4"/>
         <v>jAnn</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" ref="B56:B60" si="11">"vstacks_"&amp;VLOOKUP(A56,$S$6:$T$18,2,FALSE)&amp;"~"&amp;TEXT(O56,"0000")</f>
+        <v>vstacks_s1_d~0001</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" ref="C56:C60" si="12">H56</f>
+        <v>e 1.5 deg no OS.f3d</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" ref="H56:H60" si="13">_xlfn.TEXTJOIN(".",TRUE,I56:J56)</f>
+        <v>e 1.5 deg no OS.f3d</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" ref="J56:J60" si="14">Q56</f>
+        <v>f3d</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q56" t="str">
+        <f t="shared" ref="Q56:Q60" si="15">VLOOKUP(A56,$S$6:$U$17,3,FALSE)</f>
+        <v>f3d</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="11"/>
+        <v>vstacks_s1_d~0002</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="12"/>
+        <v>d 1.5 deg OS.f3d</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="13"/>
+        <v>d 1.5 deg OS.f3d</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="14"/>
+        <v>f3d</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q57" t="str">
+        <f t="shared" si="15"/>
+        <v>f3d</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="11"/>
+        <v>vstacks_s1_d~0003</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="12"/>
+        <v>c 2 deg (67%).f3d</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="13"/>
+        <v>c 2 deg (67%).f3d</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="14"/>
+        <v>f3d</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q58" t="str">
+        <f t="shared" si="15"/>
+        <v>f3d</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="A59">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="11"/>
+        <v>vstacks_s1_d~0004</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="12"/>
+        <v>b 2 deg (50%).f3d</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="13"/>
+        <v>b 2 deg (50%).f3d</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="14"/>
+        <v>f3d</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q59" t="str">
+        <f t="shared" si="15"/>
+        <v>f3d</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="A60">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="11"/>
+        <v>vstacks_s1_d~0005</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="12"/>
+        <v>a 3 deg.f3d</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="13"/>
+        <v>a 3 deg.f3d</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="14"/>
+        <v>f3d</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q60" t="str">
+        <f t="shared" si="15"/>
+        <v>f3d</v>
       </c>
     </row>
   </sheetData>
@@ -3494,10 +3755,10 @@
         <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -3515,7 +3776,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -3613,7 +3874,7 @@
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K3" t="s">
         <v>8</v>
@@ -3630,7 +3891,7 @@
         <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
@@ -3651,10 +3912,10 @@
         <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I5" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="K5" t="s">
         <v>81</v>
@@ -3674,7 +3935,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
@@ -3775,13 +4036,13 @@
         <v>57</v>
       </c>
       <c r="I11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K11" t="s">
         <v>141</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>142</v>
-      </c>
-      <c r="N11" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -3831,9 +4092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8EC7F-95E3-4526-8B78-C58A96098159}">
   <dimension ref="C1:K3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -3914,38 +4173,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D44EBE-400A-4EA2-9DA1-076783A77DFC}">
-  <dimension ref="A3:S6"/>
+  <dimension ref="A3:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="30.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.53125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.19921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.9296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="19" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:19" ht="17.25" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>163</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" thickTop="1" thickBot="1">
@@ -4001,10 +4242,10 @@
         <v>107</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4017,13 +4258,13 @@
       </c>
       <c r="G5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$3:$A$43)</f>
-        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
+        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,hydrogen,ELC,buildings,industry,transport,EVs,fossil,renewable,bioenergy,nuclear</v>
       </c>
       <c r="J5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="S5">
         <v>-1</v>
@@ -4031,7 +4272,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
@@ -4039,15 +4280,336 @@
       </c>
       <c r="G6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$3:$A$43)</f>
-        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
+        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,hydrogen,ELC,buildings,industry,transport,EVs,fossil,renewable,bioenergy,nuclear</v>
       </c>
       <c r="J6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="17.25" thickBot="1">
+      <c r="A10" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" thickTop="1" thickBot="1">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="str">
+        <f>H13</f>
+        <v>bioenergy,coal,gas,geothermal,hydro,hydrogen,nuclear,oil,solar,windon,windoff</v>
+      </c>
+      <c r="H13" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CName_MAP!$A$3:$A$16)</f>
+        <v>bioenergy,coal,gas,geothermal,hydro,hydrogen,nuclear,oil,solar,windon,windoff</v>
+      </c>
+      <c r="J13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M13" t="s">
+        <v>276</v>
+      </c>
+      <c r="S13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" t="str">
+        <f>B5</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="H14" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CName_MAP!$A$3:$A$16)</f>
+        <v>bioenergy,coal,gas,geothermal,hydro,hydrogen,nuclear,oil,solar,windon,windoff</v>
+      </c>
+      <c r="J14" t="s">
+        <v>161</v>
+      </c>
+      <c r="M14" t="s">
+        <v>277</v>
+      </c>
+      <c r="S14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>284</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M15" t="s">
+        <v>285</v>
+      </c>
+      <c r="S15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" t="str">
+        <f>B14</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16" t="s">
+        <v>161</v>
+      </c>
+      <c r="M16" t="s">
+        <v>286</v>
+      </c>
+      <c r="S16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="G18" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$28:$A$31)</f>
+        <v>buildings,industry,transport,EVs</v>
+      </c>
+      <c r="J18" t="s">
+        <v>161</v>
+      </c>
+      <c r="M18" t="s">
+        <v>287</v>
+      </c>
+      <c r="S18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="G19" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$28:$A$31)</f>
+        <v>buildings,industry,transport,EVs</v>
+      </c>
+      <c r="J19" t="s">
+        <v>161</v>
+      </c>
+      <c r="M19" t="s">
+        <v>288</v>
+      </c>
+      <c r="S19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="H20" t="s">
+        <v>289</v>
+      </c>
+      <c r="J20" t="s">
+        <v>161</v>
+      </c>
+      <c r="M20" t="s">
+        <v>290</v>
+      </c>
+      <c r="S20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="H21" t="s">
+        <v>289</v>
+      </c>
+      <c r="J21" t="s">
+        <v>161</v>
+      </c>
+      <c r="M21" t="s">
+        <v>291</v>
+      </c>
+      <c r="S21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="str">
+        <f>H23</f>
+        <v>hydrogen</v>
+      </c>
+      <c r="H23" t="s">
+        <v>186</v>
+      </c>
+      <c r="J23" t="s">
+        <v>161</v>
+      </c>
+      <c r="M23" t="s">
+        <v>276</v>
+      </c>
+      <c r="S23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" t="s">
+        <v>186</v>
+      </c>
+      <c r="H24" t="s">
+        <v>186</v>
+      </c>
+      <c r="J24" t="s">
+        <v>161</v>
+      </c>
+      <c r="M24" t="s">
+        <v>280</v>
+      </c>
+      <c r="S24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" t="s">
+        <v>186</v>
+      </c>
+      <c r="G25" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$3:$A$43)</f>
+        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,hydrogen,ELC,buildings,industry,transport,EVs,fossil,renewable,bioenergy,nuclear</v>
+      </c>
+      <c r="J25" t="s">
+        <v>161</v>
+      </c>
+      <c r="M25" t="s">
+        <v>292</v>
+      </c>
+      <c r="S25">
         <v>-1</v>
       </c>
     </row>
@@ -4062,7 +4624,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A47"/>
+      <selection activeCell="A12" sqref="A12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -4153,7 +4715,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -4162,7 +4724,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -4173,23 +4735,21 @@
       <c r="A12" t="s">
         <v>95</v>
       </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>Wind onshore</v>
+      <c r="B12" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>96</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>Wind offshore</v>
+      <c r="B13" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -4198,7 +4758,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -4207,7 +4767,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -4216,7 +4776,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -4225,7 +4785,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -4261,7 +4821,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -4270,7 +4830,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -4279,7 +4839,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -4288,7 +4848,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -4297,7 +4857,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -4306,7 +4866,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -4315,7 +4875,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -4324,7 +4884,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -4333,7 +4893,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -4342,7 +4902,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -4351,7 +4911,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -4360,7 +4920,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -4369,7 +4929,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -4378,7 +4938,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -4387,7 +4947,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
@@ -4396,7 +4956,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
@@ -4405,7 +4965,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
@@ -4414,7 +4974,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -4423,7 +4983,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
@@ -4432,7 +4992,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
@@ -4441,7 +5001,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
@@ -4450,7 +5010,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
@@ -4459,7 +5019,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
@@ -4468,7 +5028,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -4477,7 +5037,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -4486,7 +5046,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
@@ -4504,7 +5064,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4530,7 +5090,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B3" t="str">
         <f>A3</f>
@@ -4539,16 +5099,16 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B35" si="0">A4</f>
+        <f t="shared" ref="B4:B25" si="0">A4</f>
         <v>Elec-400V</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -4557,7 +5117,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -4566,7 +5126,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -4575,7 +5135,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -4584,7 +5144,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -4593,7 +5153,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -4602,7 +5162,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -4611,7 +5171,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -4620,7 +5180,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -4629,7 +5189,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -4638,7 +5198,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -4647,7 +5207,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -4656,7 +5216,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -4665,7 +5225,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -4674,7 +5234,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -4683,7 +5243,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -4692,7 +5252,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -4701,7 +5261,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -4710,7 +5270,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -4719,7 +5279,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -4728,7 +5288,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -4737,92 +5297,91 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>fossil</v>
+        <f t="shared" ref="B26" si="1">A26</f>
+        <v>hydrogen</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>208</v>
-      </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>renewable</v>
+        <v>188</v>
+      </c>
+      <c r="B27" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>bioenergy</v>
+        <f t="shared" ref="B28:B35" si="2">A28</f>
+        <v>buildings</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>hydrogen</v>
+        <f t="shared" si="2"/>
+        <v>industry</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>nuclear</v>
+        <f t="shared" si="2"/>
+        <v>transport</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>ELC</v>
+        <f t="shared" si="2"/>
+        <v>EVs</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>192</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>buildings</v>
+      <c r="A32" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B32" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>fossil</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>industry</v>
+      <c r="A33" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>renewable</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>transport</v>
+      <c r="A34" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>bioenergy</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>195</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>EVs</v>
+      <c r="A35" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>nuclear</v>
       </c>
     </row>
   </sheetData>
@@ -4833,11 +5392,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -4862,6 +5421,103 @@
       </c>
       <c r="C2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A3</f>
+        <v>bioenergy</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B11" si="0">A4</f>
+        <v>coal</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>gas</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>geothermal</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>hydro</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>hydrogen</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>nuclear</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>oil</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>solar</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -4888,7 +5544,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4904,32 +5560,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
         <v>147</v>
-      </c>
-      <c r="C3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
         <v>151</v>
-      </c>
-      <c r="B5" t="s">
-        <v>152</v>
       </c>
       <c r="C5" t="str">
         <f>LEFT(B5,2)</f>
@@ -4938,10 +5594,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
@@ -4950,10 +5606,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4962,10 +5618,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4974,10 +5630,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -4986,10 +5642,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -5006,7 +5662,8 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5162,7 +5819,7 @@
         <v>Bio Power</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5174,7 +5831,7 @@
         <v>Solar Util</v>
       </c>
       <c r="D13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5210,7 +5867,7 @@
         <v>Geothermal P</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5222,7 +5879,7 @@
         <v>Hydro Dam</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5234,7 +5891,7 @@
         <v>Hydro RoR</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5246,7 +5903,7 @@
         <v>Nuclear P</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5258,7 +5915,7 @@
         <v>Nuclear SMR</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5306,7 +5963,7 @@
         <v>Demand</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5318,7 +5975,7 @@
         <v>Transformers Dn</v>
       </c>
       <c r="D25" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5330,7 +5987,7 @@
         <v>Transformers Up</v>
       </c>
       <c r="D26" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5342,7 +5999,7 @@
         <v>Grid-220V</v>
       </c>
       <c r="D27" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5354,7 +6011,7 @@
         <v>Grid-400V</v>
       </c>
       <c r="D28" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5366,7 +6023,7 @@
         <v>Grid-380V</v>
       </c>
       <c r="D29" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5378,7 +6035,7 @@
         <v>Grid-225V</v>
       </c>
       <c r="D30" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5390,7 +6047,7 @@
         <v>Grid-330V</v>
       </c>
       <c r="D31" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5402,7 +6059,7 @@
         <v>Grid-275V</v>
       </c>
       <c r="D32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5414,7 +6071,7 @@
         <v>Grid-420V</v>
       </c>
       <c r="D33" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5426,7 +6083,7 @@
         <v>Grid-300V</v>
       </c>
       <c r="D34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5438,7 +6095,7 @@
         <v>Grid-500V</v>
       </c>
       <c r="D35" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5450,7 +6107,7 @@
         <v>Grid-750V</v>
       </c>
       <c r="D36" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5462,7 +6119,7 @@
         <v>Grid-450V</v>
       </c>
       <c r="D37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5474,7 +6131,7 @@
         <v>Grid-515V</v>
       </c>
       <c r="D38" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -5486,7 +6143,7 @@
         <v>Grid-525V</v>
       </c>
       <c r="D39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -5498,7 +6155,7 @@
         <v>Grid-320V</v>
       </c>
       <c r="D40" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -5510,7 +6167,7 @@
         <v>Grid-150V</v>
       </c>
       <c r="D41" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -5522,7 +6179,7 @@
         <v>Grid-270V</v>
       </c>
       <c r="D42" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -5534,7 +6191,7 @@
         <v>Grid-350V</v>
       </c>
       <c r="D43" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -5546,7 +6203,7 @@
         <v>Grid-250V</v>
       </c>
       <c r="D44" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -5558,7 +6215,7 @@
         <v>Grid-200V</v>
       </c>
       <c r="D45" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -5570,7 +6227,7 @@
         <v>Grid-236V</v>
       </c>
       <c r="D46" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -5582,7 +6239,7 @@
         <v>Grid-600V</v>
       </c>
       <c r="D47" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -5594,10 +6251,10 @@
         <v>Aggregators</v>
       </c>
       <c r="D48" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -5606,43 +6263,43 @@
         <v>DUMMY_IMP</v>
       </c>
       <c r="D49" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>70</v>
       </c>
+      <c r="B50" t="s">
+        <v>263</v>
+      </c>
       <c r="C50" t="s">
         <v>133</v>
       </c>
       <c r="E50" t="s">
         <v>137</v>
       </c>
-      <c r="F50" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>70</v>
       </c>
+      <c r="B51" t="s">
+        <v>263</v>
+      </c>
       <c r="C51" t="s">
         <v>134</v>
       </c>
       <c r="E51" t="s">
         <v>138</v>
       </c>
-      <c r="F51" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
         <v>135</v>
@@ -5651,12 +6308,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C53" t="s">
         <v>136</v>
@@ -5665,7 +6322,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -5676,7 +6333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -5687,7 +6344,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>70</v>
       </c>

</xml_diff>